<commit_message>
added excel files and change model of entry
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/LOANS PYBLE_RCVBL.xlsx
+++ b/aCCTg. pROGRAm/LOANS PYBLE_RCVBL.xlsx
@@ -27,9 +27,6 @@
     <t>CR</t>
   </si>
   <si>
-    <t>L/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">      CASH</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>LOAN AVAILMENT/RECEIVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -239,10 +239,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="17"/>
+      <c r="E4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -672,7 +672,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8">
         <v>50000</v>
@@ -708,7 +708,7 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8">
@@ -721,7 +721,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="8">
         <v>1500</v>
@@ -757,7 +757,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14">
@@ -770,14 +770,14 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="17"/>
+      <c r="C22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="16"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -887,7 +887,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="8">
         <v>100000</v>
@@ -909,7 +909,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8">
@@ -940,7 +940,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -963,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="8">
         <v>5000</v>
@@ -985,7 +985,7 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8">
@@ -1007,7 +1007,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed payment to account receivable display, catched errors
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/LOANS PYBLE_RCVBL.xlsx
+++ b/aCCTg. pROGRAm/LOANS PYBLE_RCVBL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="14355" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,11 +220,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -549,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,448 +561,445 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>50000</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7">
         <f>+D15</f>
         <v>50000</v>
       </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>50000</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="8">
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7">
+        <f>+D19</f>
+        <v>1500</v>
+      </c>
+      <c r="E8" s="7">
         <f>+C17</f>
         <v>1500</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="8">
-        <f>+D19</f>
-        <v>1500</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="10">
-        <f>-F6+E7</f>
-        <v>-48500</v>
-      </c>
-      <c r="G8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="10">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9">
         <f>+C7-D8</f>
         <v>48500</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="9">
+        <f>-F7+E8</f>
+        <v>-48500</v>
+      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>1</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>50000</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7">
         <f>+C13</f>
         <v>50000</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>2</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>1500</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13">
         <v>1500</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="15"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="16" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="8">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7">
         <f>+D32</f>
         <v>100000</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <f>+C30</f>
         <v>100000</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7">
+      <c r="F24" s="5"/>
+      <c r="G24" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6">
-        <v>2</v>
-      </c>
-      <c r="C25" s="10">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9">
         <f>+C37</f>
         <v>5000</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <f>+D24-C25</f>
         <v>95000</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8">
+      <c r="E25" s="5"/>
+      <c r="F25" s="7">
         <f>+D39</f>
         <v>5000</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>100000</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7">
         <f>+C30</f>
         <v>100000</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="7"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>2</v>
-      </c>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>5000</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="7"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7">
         <f>+C37</f>
         <v>5000</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="7"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="15"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -1065,10 +1061,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>